<commit_message>
Notes atuo sync: from windows.
</commit_message>
<xml_diff>
--- a/ComputerArchitecture/cpu/PL.xlsx
+++ b/ComputerArchitecture/cpu/PL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\workpath\Notes\ComputerArchitecture\cpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4884D82-3DD9-42FF-8912-5C04787DF374}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36071979-B2F0-4875-80CC-D163CD3F5918}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9024" firstSheet="1" activeTab="1" xr2:uid="{4A1BF099-32EC-4A84-8481-4666D932E36A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9024" activeTab="1" xr2:uid="{4A1BF099-32EC-4A84-8481-4666D932E36A}"/>
   </bookViews>
   <sheets>
     <sheet name="PIPELINE DESIGN" sheetId="7" r:id="rId1"/>
@@ -2006,34 +2006,25 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="6" xfId="3" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="14" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="4">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="14" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2051,17 +2042,26 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="14" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="14" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="4">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2381,6 +2381,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7010006C-474D-4AEC-BC38-B38BF708AA26}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -2390,8 +2393,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="46" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" style="46" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="30" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" style="30" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" customWidth="1"/>
@@ -2400,7 +2403,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="30" t="s">
         <v>301</v>
       </c>
       <c r="C1" s="28" t="s">
@@ -2435,411 +2438,411 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="30" t="s">
         <v>310</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="D2" s="48">
-        <v>1</v>
-      </c>
-      <c r="E2" s="48">
-        <v>1</v>
-      </c>
-      <c r="F2" s="48">
-        <v>1</v>
-      </c>
-      <c r="G2" s="48">
-        <v>1</v>
-      </c>
-      <c r="H2" s="48">
-        <v>1</v>
-      </c>
-      <c r="I2" s="48">
-        <v>1</v>
-      </c>
-      <c r="J2" s="48">
-        <v>1</v>
-      </c>
-      <c r="K2" s="48" t="s">
+      <c r="D2" s="31">
+        <v>1</v>
+      </c>
+      <c r="E2" s="31">
+        <v>1</v>
+      </c>
+      <c r="F2" s="31">
+        <v>1</v>
+      </c>
+      <c r="G2" s="31">
+        <v>1</v>
+      </c>
+      <c r="H2" s="31">
+        <v>1</v>
+      </c>
+      <c r="I2" s="31">
+        <v>1</v>
+      </c>
+      <c r="J2" s="31">
+        <v>1</v>
+      </c>
+      <c r="K2" s="31" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
-      <c r="B3" s="46" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="30" t="s">
         <v>354</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="D3" s="48">
-        <v>1</v>
-      </c>
-      <c r="E3" s="48">
+      <c r="D3" s="31">
+        <v>1</v>
+      </c>
+      <c r="E3" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="46" t="s">
+      <c r="A4" s="32"/>
+      <c r="B4" s="30" t="s">
         <v>311</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="D4" s="48">
-        <v>1</v>
-      </c>
-      <c r="E4" s="48">
-        <v>1</v>
-      </c>
-      <c r="F4" s="48">
-        <v>1</v>
-      </c>
-      <c r="G4" s="48">
-        <v>1</v>
-      </c>
-      <c r="H4" s="48">
-        <v>1</v>
-      </c>
-      <c r="I4" s="48">
-        <v>1</v>
-      </c>
-      <c r="J4" s="48">
-        <v>1</v>
-      </c>
-      <c r="K4" s="48">
+      <c r="D4" s="31">
+        <v>1</v>
+      </c>
+      <c r="E4" s="31">
+        <v>1</v>
+      </c>
+      <c r="F4" s="31">
+        <v>1</v>
+      </c>
+      <c r="G4" s="31">
+        <v>1</v>
+      </c>
+      <c r="H4" s="31">
+        <v>1</v>
+      </c>
+      <c r="I4" s="31">
+        <v>1</v>
+      </c>
+      <c r="J4" s="31">
+        <v>1</v>
+      </c>
+      <c r="K4" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="48" t="s">
+      <c r="A5" s="32"/>
+      <c r="B5" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="D5" s="48">
-        <v>1</v>
-      </c>
-      <c r="E5" s="48">
+      <c r="D5" s="31">
+        <v>1</v>
+      </c>
+      <c r="E5" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="46" t="s">
+      <c r="A6" s="32"/>
+      <c r="B6" s="30" t="s">
         <v>312</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="D6" s="48">
-        <v>1</v>
-      </c>
-      <c r="E6" s="48">
-        <v>1</v>
-      </c>
-      <c r="F6" s="48">
-        <v>1</v>
-      </c>
-      <c r="G6" s="48">
-        <v>1</v>
-      </c>
-      <c r="H6" s="48">
-        <v>1</v>
-      </c>
-      <c r="I6" s="48">
-        <v>1</v>
-      </c>
-      <c r="J6" s="48">
-        <v>1</v>
-      </c>
-      <c r="K6" s="48">
+      <c r="D6" s="31">
+        <v>1</v>
+      </c>
+      <c r="E6" s="31">
+        <v>1</v>
+      </c>
+      <c r="F6" s="31">
+        <v>1</v>
+      </c>
+      <c r="G6" s="31">
+        <v>1</v>
+      </c>
+      <c r="H6" s="31">
+        <v>1</v>
+      </c>
+      <c r="I6" s="31">
+        <v>1</v>
+      </c>
+      <c r="J6" s="31">
+        <v>1</v>
+      </c>
+      <c r="K6" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="46" t="s">
+      <c r="A7" s="32"/>
+      <c r="B7" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="D7" s="48">
-        <v>1</v>
-      </c>
-      <c r="E7" s="48">
-        <v>1</v>
-      </c>
-      <c r="F7" s="48">
-        <v>1</v>
-      </c>
-      <c r="G7" s="48">
-        <v>1</v>
-      </c>
-      <c r="H7" s="48">
-        <v>1</v>
-      </c>
-      <c r="I7" s="48">
-        <v>1</v>
-      </c>
-      <c r="J7" s="48">
-        <v>1</v>
-      </c>
-      <c r="K7" s="48">
+      <c r="D7" s="31">
+        <v>1</v>
+      </c>
+      <c r="E7" s="31">
+        <v>1</v>
+      </c>
+      <c r="F7" s="31">
+        <v>1</v>
+      </c>
+      <c r="G7" s="31">
+        <v>1</v>
+      </c>
+      <c r="H7" s="31">
+        <v>1</v>
+      </c>
+      <c r="I7" s="31">
+        <v>1</v>
+      </c>
+      <c r="J7" s="31">
+        <v>1</v>
+      </c>
+      <c r="K7" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="46" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="30" t="s">
         <v>314</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="D8" s="48">
-        <v>1</v>
-      </c>
-      <c r="E8" s="48">
-        <v>1</v>
-      </c>
-      <c r="F8" s="48">
-        <v>1</v>
-      </c>
-      <c r="G8" s="48">
-        <v>1</v>
-      </c>
-      <c r="H8" s="48">
-        <v>1</v>
-      </c>
-      <c r="I8" s="48">
-        <v>1</v>
-      </c>
-      <c r="J8" s="48">
-        <v>1</v>
-      </c>
-      <c r="K8" s="48">
+      <c r="D8" s="31">
+        <v>1</v>
+      </c>
+      <c r="E8" s="31">
+        <v>1</v>
+      </c>
+      <c r="F8" s="31">
+        <v>1</v>
+      </c>
+      <c r="G8" s="31">
+        <v>1</v>
+      </c>
+      <c r="H8" s="31">
+        <v>1</v>
+      </c>
+      <c r="I8" s="31">
+        <v>1</v>
+      </c>
+      <c r="J8" s="31">
+        <v>1</v>
+      </c>
+      <c r="K8" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="46" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="D9" s="48">
-        <v>1</v>
-      </c>
-      <c r="E9" s="48">
-        <v>1</v>
-      </c>
-      <c r="F9" s="48">
-        <v>1</v>
-      </c>
-      <c r="G9" s="48">
-        <v>1</v>
-      </c>
-      <c r="H9" s="48">
-        <v>1</v>
-      </c>
-      <c r="I9" s="48">
-        <v>1</v>
-      </c>
-      <c r="J9" s="48">
-        <v>1</v>
-      </c>
-      <c r="K9" s="48">
+      <c r="D9" s="31">
+        <v>1</v>
+      </c>
+      <c r="E9" s="31">
+        <v>1</v>
+      </c>
+      <c r="F9" s="31">
+        <v>1</v>
+      </c>
+      <c r="G9" s="31">
+        <v>1</v>
+      </c>
+      <c r="H9" s="31">
+        <v>1</v>
+      </c>
+      <c r="I9" s="31">
+        <v>1</v>
+      </c>
+      <c r="J9" s="31">
+        <v>1</v>
+      </c>
+      <c r="K9" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="46" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="D10" s="48">
-        <v>1</v>
-      </c>
-      <c r="E10" s="48">
+      <c r="D10" s="31">
+        <v>1</v>
+      </c>
+      <c r="E10" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="30" t="s">
         <v>323</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="30" t="s">
         <v>326</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F11" s="48">
+      <c r="F11" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="E12" s="48" t="s">
+      <c r="E12" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F12" s="48">
+      <c r="F12" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="30" t="s">
         <v>328</v>
       </c>
-      <c r="E13" s="48" t="s">
+      <c r="E13" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F13" s="48">
+      <c r="F13" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="30" t="s">
         <v>331</v>
       </c>
-      <c r="E14" s="48" t="s">
+      <c r="E14" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F14" s="48">
-        <v>1</v>
-      </c>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48">
-        <v>1</v>
-      </c>
-      <c r="I14" s="48">
+      <c r="F14" s="31">
+        <v>1</v>
+      </c>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31">
+        <v>1</v>
+      </c>
+      <c r="I14" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="30" t="s">
         <v>325</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F15" s="48">
-        <v>1</v>
-      </c>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48">
-        <v>1</v>
-      </c>
-      <c r="I15" s="48">
+      <c r="F15" s="31">
+        <v>1</v>
+      </c>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31">
+        <v>1</v>
+      </c>
+      <c r="I15" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="30" t="s">
         <v>352</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F16" s="48">
-        <v>1</v>
-      </c>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48">
-        <v>1</v>
-      </c>
-      <c r="I16" s="48">
+      <c r="F16" s="31">
+        <v>1</v>
+      </c>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31">
+        <v>1</v>
+      </c>
+      <c r="I16" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="30" t="s">
         <v>324</v>
       </c>
-      <c r="E17" s="48" t="s">
+      <c r="E17" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F17" s="48">
-        <v>1</v>
-      </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48">
-        <v>1</v>
-      </c>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48">
-        <v>1</v>
-      </c>
-      <c r="K17" s="48" t="s">
+      <c r="F17" s="31">
+        <v>1</v>
+      </c>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31">
+        <v>1</v>
+      </c>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31">
+        <v>1</v>
+      </c>
+      <c r="K17" s="31" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="30" t="s">
         <v>333</v>
       </c>
-      <c r="E18" s="48" t="s">
+      <c r="E18" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F18" s="48">
-        <v>1</v>
-      </c>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48">
-        <v>1</v>
-      </c>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48">
+      <c r="F18" s="31">
+        <v>1</v>
+      </c>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31">
+        <v>1</v>
+      </c>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="30" t="s">
         <v>332</v>
       </c>
-      <c r="E19" s="48" t="s">
+      <c r="E19" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F19" s="48">
-        <v>1</v>
-      </c>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48">
-        <v>1</v>
-      </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48">
-        <v>1</v>
-      </c>
-      <c r="K19" s="48" t="s">
+      <c r="F19" s="31">
+        <v>1</v>
+      </c>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31">
+        <v>1</v>
+      </c>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31">
+        <v>1</v>
+      </c>
+      <c r="K19" s="31" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="30" t="s">
         <v>334</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="48" t="s">
+      <c r="E20" s="31" t="s">
         <v>341</v>
       </c>
       <c r="F20" t="s">
@@ -2847,10 +2850,10 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="31" t="s">
         <v>341</v>
       </c>
       <c r="F21" t="s">
@@ -2858,10 +2861,10 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="48" t="s">
+      <c r="E22" s="31" t="s">
         <v>341</v>
       </c>
       <c r="F22" t="s">
@@ -2869,10 +2872,10 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="48" t="s">
+      <c r="E23" s="31" t="s">
         <v>341</v>
       </c>
       <c r="F23" t="s">
@@ -2880,10 +2883,10 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="48" t="s">
+      <c r="E24" s="31" t="s">
         <v>341</v>
       </c>
       <c r="F24" t="s">
@@ -2891,43 +2894,43 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="E25" s="48" t="s">
+      <c r="E25" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F25" s="48">
+      <c r="F25" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="E26" s="48" t="s">
+      <c r="E26" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F26" s="48">
+      <c r="F26" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="30" t="s">
         <v>319</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F27" s="48">
+      <c r="F27" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="E28" s="48" t="s">
+      <c r="E28" s="31" t="s">
         <v>341</v>
       </c>
       <c r="F28" t="s">
@@ -2935,48 +2938,48 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="E29" s="48" t="s">
+      <c r="E29" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F29" s="48">
-        <v>1</v>
-      </c>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="48"/>
+      <c r="F29" s="31">
+        <v>1</v>
+      </c>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="30" t="s">
         <v>329</v>
       </c>
-      <c r="E30" s="48" t="s">
+      <c r="E30" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F30" s="48">
+      <c r="F30" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="30" t="s">
         <v>330</v>
       </c>
-      <c r="E31" s="48" t="s">
+      <c r="E31" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F31" s="48">
+      <c r="F31" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="30" t="s">
         <v>344</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="31" t="s">
         <v>341</v>
       </c>
       <c r="F32" t="s">
@@ -2984,10 +2987,10 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="30" t="s">
         <v>343</v>
       </c>
-      <c r="E33" s="48" t="s">
+      <c r="E33" s="31" t="s">
         <v>341</v>
       </c>
       <c r="F33" t="s">
@@ -2995,77 +2998,77 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="46" t="s">
+      <c r="B34" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="G34" s="48" t="s">
+      <c r="G34" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="H34" s="48">
-        <v>1</v>
-      </c>
-      <c r="I34" s="48">
-        <v>1</v>
-      </c>
-      <c r="J34" s="48">
-        <v>1</v>
-      </c>
-      <c r="K34" s="48">
+      <c r="H34" s="31">
+        <v>1</v>
+      </c>
+      <c r="I34" s="31">
+        <v>1</v>
+      </c>
+      <c r="J34" s="31">
+        <v>1</v>
+      </c>
+      <c r="K34" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="30" t="s">
         <v>345</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="30" t="s">
         <v>346</v>
       </c>
-      <c r="E35" s="48" t="s">
+      <c r="E35" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F35" s="46" t="s">
+      <c r="F35" s="30" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="30" t="s">
         <v>347</v>
       </c>
-      <c r="E36" s="48" t="s">
+      <c r="E36" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="F36" s="46" t="s">
+      <c r="F36" s="30" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="G37" s="48" t="s">
+      <c r="G37" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="H37" s="46" t="s">
+      <c r="H37" s="30" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="30" t="s">
         <v>349</v>
       </c>
-      <c r="I38" s="48" t="s">
+      <c r="I38" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="J38" s="46" t="s">
+      <c r="J38" s="30" t="s">
         <v>349</v>
       </c>
-      <c r="K38" s="48" t="s">
+      <c r="K38" s="31" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="30" t="s">
         <v>350</v>
       </c>
       <c r="C39" s="28"/>
@@ -3080,7 +3083,7 @@
       <c r="L39" s="28"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="46" t="s">
+      <c r="B40" s="30" t="s">
         <v>351</v>
       </c>
       <c r="C40" s="28"/>
@@ -3095,51 +3098,51 @@
       <c r="L40" s="28"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="30" t="s">
         <v>336</v>
       </c>
-      <c r="B41" s="46" t="s">
+      <c r="B41" s="30" t="s">
         <v>337</v>
       </c>
-      <c r="H41" s="46" t="s">
+      <c r="H41" s="30" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="30" t="s">
         <v>340</v>
       </c>
-      <c r="J42" s="46" t="s">
+      <c r="J42" s="30" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="46" t="s">
+      <c r="B43" s="30" t="s">
         <v>338</v>
       </c>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="46" t="s">
+      <c r="B44" s="30" t="s">
         <v>339</v>
       </c>
-      <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="30" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="30" t="s">
         <v>355</v>
       </c>
     </row>
@@ -3149,16 +3152,19 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="68" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A07C5C0-AD03-4360-B448-7E7DEFEACDFB}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F34" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3172,26 +3178,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="42" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="39" t="s">
         <v>173</v>
       </c>
       <c r="K1" s="24"/>
@@ -3209,48 +3215,48 @@
       <c r="W1" s="13"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33" t="s">
         <v>127</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="J2" s="43"/>
-      <c r="K2" s="39" t="s">
+      <c r="J2" s="40"/>
+      <c r="K2" s="34" t="s">
         <v>284</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="39" t="s">
+      <c r="L2" s="35"/>
+      <c r="M2" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="39" t="s">
+      <c r="N2" s="36"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="39" t="s">
+      <c r="Q2" s="36"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T2" s="34"/>
+      <c r="T2" s="35"/>
       <c r="U2" s="13"/>
       <c r="V2" s="13"/>
       <c r="W2" s="13"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="20" t="s">
         <v>128</v>
       </c>
@@ -3260,8 +3266,8 @@
       <c r="H3" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="44"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="41"/>
       <c r="K3" s="20" t="s">
         <v>252</v>
       </c>
@@ -5598,21 +5604,22 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:I1"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="M2:O2"/>
     <mergeCell ref="P2:R2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:J3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="44" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5631,26 +5638,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="42" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="39" t="s">
         <v>173</v>
       </c>
       <c r="K1" s="23" t="s">
@@ -5669,10 +5676,10 @@
       <c r="V1" s="24"/>
       <c r="W1" s="24"/>
       <c r="X1" s="24"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="34"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="35"/>
       <c r="AC1" s="14"/>
       <c r="AD1" s="29" t="s">
         <v>297</v>
@@ -5688,47 +5695,47 @@
       </c>
     </row>
     <row r="2" spans="1:33" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33" t="s">
         <v>127</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="J2" s="43"/>
+      <c r="J2" s="40"/>
       <c r="K2" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="34" t="s">
         <v>283</v>
       </c>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="39" t="s">
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="34" t="s">
         <v>284</v>
       </c>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="39" t="s">
+      <c r="Q2" s="35"/>
+      <c r="R2" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="39" t="s">
+      <c r="S2" s="35"/>
+      <c r="T2" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="U2" s="33"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="39" t="s">
+      <c r="U2" s="36"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="34"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="35"/>
       <c r="Z2" s="23" t="s">
         <v>286</v>
       </c>
@@ -5741,11 +5748,11 @@
       <c r="AG2" s="15"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="20" t="s">
         <v>128</v>
       </c>
@@ -5755,8 +5762,8 @@
       <c r="H3" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="44"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="41"/>
       <c r="K3" s="19" t="s">
         <v>288</v>
       </c>
@@ -5834,13 +5841,13 @@
       <c r="J4" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="K4" s="30" t="s">
+      <c r="K4" s="42" t="s">
         <v>287</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="L4" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="M4" s="35" t="s">
+      <c r="M4" s="45" t="s">
         <v>129</v>
       </c>
       <c r="N4" s="13"/>
@@ -5907,9 +5914,9 @@
       <c r="J5" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
       <c r="P5" s="13" t="s">
@@ -5972,9 +5979,9 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
       <c r="P6" s="13" t="s">
@@ -6037,9 +6044,9 @@
       <c r="J7" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13" t="s">
@@ -6100,9 +6107,9 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
       <c r="P8" s="13" t="s">
@@ -6165,9 +6172,9 @@
       <c r="J9" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="K9" s="31"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13" t="s">
@@ -6226,9 +6233,9 @@
       <c r="J10" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="K10" s="31"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13" t="s">
@@ -6287,9 +6294,9 @@
       <c r="J11" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="K11" s="31"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13" t="s">
@@ -6346,9 +6353,9 @@
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13" t="s">
@@ -6405,9 +6412,9 @@
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13" t="s">
@@ -6464,9 +6471,9 @@
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
       <c r="P14" s="13" t="s">
@@ -6521,9 +6528,9 @@
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
       <c r="P15" s="13" t="s">
@@ -6578,9 +6585,9 @@
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
       <c r="P16" s="13" t="s">
@@ -6639,9 +6646,9 @@
       <c r="J17" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="K17" s="31"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="13" t="s">
@@ -6698,9 +6705,9 @@
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
       <c r="N18" s="13"/>
       <c r="O18" s="13"/>
       <c r="P18" s="13" t="s">
@@ -6755,9 +6762,9 @@
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
       <c r="P19" s="13" t="s">
@@ -6812,9 +6819,9 @@
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
       <c r="P20" s="13" t="s">
@@ -6867,9 +6874,9 @@
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
       <c r="N21" s="13"/>
       <c r="O21" s="13"/>
       <c r="P21" s="13" t="s">
@@ -6922,9 +6929,9 @@
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
       <c r="N22" s="13"/>
       <c r="O22" s="13"/>
       <c r="P22" s="13" t="s">
@@ -6979,9 +6986,9 @@
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
       <c r="P23" s="13" t="s">
@@ -7036,9 +7043,9 @@
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
       <c r="N24" s="13"/>
       <c r="O24" s="13"/>
       <c r="P24" s="13" t="s">
@@ -7091,9 +7098,9 @@
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
       <c r="N25" s="13"/>
       <c r="O25" s="13"/>
       <c r="P25" s="13" t="s">
@@ -7150,9 +7157,9 @@
       <c r="J26" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="K26" s="31"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
       <c r="N26" s="13"/>
       <c r="O26" s="13"/>
       <c r="P26" s="13" t="s">
@@ -7207,9 +7214,9 @@
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
       <c r="P27" s="13" t="s">
@@ -7268,9 +7275,9 @@
         <v>154</v>
       </c>
       <c r="J28" s="13"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="36"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
       <c r="N28" s="13"/>
       <c r="O28" s="13"/>
       <c r="P28" s="13" t="s">
@@ -7327,9 +7334,9 @@
         <v>159</v>
       </c>
       <c r="J29" s="13"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
       <c r="N29" s="13"/>
       <c r="O29" s="13"/>
       <c r="P29" s="13" t="s">
@@ -7388,9 +7395,9 @@
         <v>11</v>
       </c>
       <c r="J30" s="13"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="36"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
       <c r="N30" s="13"/>
       <c r="O30" s="13"/>
       <c r="P30" s="13" t="s">
@@ -7451,9 +7458,9 @@
         <v>61</v>
       </c>
       <c r="J31" s="13"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
       <c r="N31" s="13"/>
       <c r="O31" s="13"/>
       <c r="P31" s="13" t="s">
@@ -7510,9 +7517,9 @@
       <c r="J32" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K32" s="31"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
       <c r="N32" s="13"/>
       <c r="O32" s="13"/>
       <c r="P32" s="13" t="s">
@@ -7571,9 +7578,9 @@
       <c r="J33" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="K33" s="31"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="36"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
       <c r="N33" s="13"/>
       <c r="O33" s="13"/>
       <c r="P33" s="13" t="s">
@@ -7630,9 +7637,9 @@
         <v>230</v>
       </c>
       <c r="J34" s="13"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="36"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="46"/>
+      <c r="M34" s="46"/>
       <c r="N34" s="13"/>
       <c r="O34" s="13"/>
       <c r="P34" s="13" t="s">
@@ -7689,9 +7696,9 @@
         <v>209</v>
       </c>
       <c r="J35" s="13"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="46"/>
       <c r="N35" s="13"/>
       <c r="O35" s="13"/>
       <c r="P35" s="13" t="s">
@@ -7750,9 +7757,9 @@
       <c r="J36" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="K36" s="31"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="36"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="46"/>
       <c r="N36" s="13"/>
       <c r="O36" s="13"/>
       <c r="P36" s="13" t="s">
@@ -7811,9 +7818,9 @@
       <c r="J37" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="K37" s="31"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="36"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="46"/>
       <c r="N37" s="13"/>
       <c r="O37" s="13"/>
       <c r="P37" s="13" t="s">
@@ -7870,9 +7877,9 @@
         <v>250</v>
       </c>
       <c r="J38" s="13"/>
-      <c r="K38" s="31"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="36"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
       <c r="N38" s="13"/>
       <c r="O38" s="13"/>
       <c r="P38" s="13" t="s">
@@ -7927,9 +7934,9 @@
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
-      <c r="K39" s="31"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="46"/>
       <c r="N39" s="13"/>
       <c r="O39" s="13"/>
       <c r="P39" s="13" t="s">
@@ -7984,9 +7991,9 @@
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="36"/>
+      <c r="K40" s="43"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
       <c r="N40" s="13"/>
       <c r="O40" s="13"/>
       <c r="P40" s="13" t="s">
@@ -8043,9 +8050,9 @@
         <v>257</v>
       </c>
       <c r="J41" s="13"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="36"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="46"/>
       <c r="N41" s="13"/>
       <c r="O41" s="13"/>
       <c r="P41" s="13" t="s">
@@ -8104,9 +8111,9 @@
       <c r="J42" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="K42" s="31"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="36"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="46"/>
       <c r="N42" s="13"/>
       <c r="O42" s="13"/>
       <c r="P42" s="13" t="s">
@@ -8165,9 +8172,9 @@
       <c r="J43" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="K43" s="31"/>
-      <c r="L43" s="36"/>
-      <c r="M43" s="36"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="46"/>
+      <c r="M43" s="46"/>
       <c r="N43" s="13"/>
       <c r="O43" s="13"/>
       <c r="P43" s="13" t="s">
@@ -8226,9 +8233,9 @@
       <c r="J44" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="K44" s="31"/>
-      <c r="L44" s="36"/>
-      <c r="M44" s="36"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="46"/>
+      <c r="M44" s="46"/>
       <c r="N44" s="13"/>
       <c r="O44" s="13"/>
       <c r="P44" s="13" t="s">
@@ -8287,9 +8294,9 @@
       <c r="J45" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="K45" s="31"/>
-      <c r="L45" s="36"/>
-      <c r="M45" s="36"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="46"/>
+      <c r="M45" s="46"/>
       <c r="N45" s="13"/>
       <c r="O45" s="13"/>
       <c r="P45" s="13" t="s">
@@ -8346,9 +8353,9 @@
         <v>213</v>
       </c>
       <c r="J46" s="13"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="36"/>
-      <c r="M46" s="36"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="46"/>
+      <c r="M46" s="46"/>
       <c r="N46" s="13"/>
       <c r="O46" s="13"/>
       <c r="P46" s="13" t="s">
@@ -8405,9 +8412,9 @@
         <v>220</v>
       </c>
       <c r="J47" s="13"/>
-      <c r="K47" s="31"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="36"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="46"/>
+      <c r="M47" s="46"/>
       <c r="N47" s="13"/>
       <c r="O47" s="13"/>
       <c r="P47" s="13" t="s">
@@ -8456,9 +8463,9 @@
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
-      <c r="K48" s="31"/>
-      <c r="L48" s="36"/>
-      <c r="M48" s="36"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="46"/>
+      <c r="M48" s="46"/>
       <c r="N48" s="13"/>
       <c r="O48" s="13"/>
       <c r="P48" s="13"/>
@@ -8493,9 +8500,9 @@
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="37"/>
-      <c r="M49" s="37"/>
+      <c r="K49" s="44"/>
+      <c r="L49" s="47"/>
+      <c r="M49" s="47"/>
       <c r="N49" s="13"/>
       <c r="O49" s="13"/>
       <c r="P49" s="13"/>
@@ -8718,6 +8725,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:I1"/>
     <mergeCell ref="K4:K49"/>
     <mergeCell ref="L4:L49"/>
     <mergeCell ref="M4:M49"/>
@@ -8729,11 +8741,6 @@
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="T2:V2"/>
     <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:J3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -8804,26 +8811,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="42" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="39" t="s">
         <v>173</v>
       </c>
       <c r="K1" s="23" t="s">
@@ -8842,10 +8849,10 @@
       <c r="V1" s="24"/>
       <c r="W1" s="24"/>
       <c r="X1" s="24"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="34"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="35"/>
       <c r="AC1" s="14"/>
       <c r="AD1" s="29" t="s">
         <v>297</v>
@@ -8861,47 +8868,47 @@
       </c>
     </row>
     <row r="2" spans="1:35" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33" t="s">
         <v>127</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="J2" s="43"/>
+      <c r="J2" s="40"/>
       <c r="K2" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="34" t="s">
         <v>283</v>
       </c>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="39" t="s">
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="34" t="s">
         <v>284</v>
       </c>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="39" t="s">
+      <c r="Q2" s="35"/>
+      <c r="R2" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="39" t="s">
+      <c r="S2" s="35"/>
+      <c r="T2" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="U2" s="33"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="39" t="s">
+      <c r="U2" s="36"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="34"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="35"/>
       <c r="Z2" s="23" t="s">
         <v>286</v>
       </c>
@@ -8916,11 +8923,11 @@
       <c r="AI2" s="15"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="20" t="s">
         <v>128</v>
       </c>
@@ -8930,8 +8937,8 @@
       <c r="H3" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="44"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="41"/>
       <c r="K3" s="19" t="s">
         <v>288</v>
       </c>
@@ -8999,13 +9006,13 @@
       <c r="J4" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="K4" s="30" t="s">
+      <c r="K4" s="42" t="s">
         <v>287</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="L4" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="M4" s="35" t="s">
+      <c r="M4" s="45" t="s">
         <v>129</v>
       </c>
       <c r="P4" s="13" t="s">
@@ -9061,9 +9068,9 @@
       <c r="J5" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
       <c r="P5" s="13" t="s">
         <v>145</v>
       </c>
@@ -9114,9 +9121,9 @@
       <c r="E6" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
       <c r="P6" s="13" t="s">
         <v>145</v>
       </c>
@@ -9167,9 +9174,9 @@
       <c r="J7" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
       <c r="P7" s="13" t="s">
         <v>145</v>
       </c>
@@ -9217,9 +9224,9 @@
       <c r="E8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="31"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
       <c r="P8" s="13" t="s">
         <v>145</v>
       </c>
@@ -9270,9 +9277,9 @@
       <c r="J9" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="K9" s="31"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
       <c r="P9" s="13" t="s">
         <v>151</v>
       </c>
@@ -9318,9 +9325,9 @@
       <c r="J10" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="K10" s="31"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
       <c r="P10" s="13" t="s">
         <v>163</v>
       </c>
@@ -9366,9 +9373,9 @@
       <c r="J11" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="K11" s="31"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
       <c r="P11" s="13" t="s">
         <v>151</v>
       </c>
@@ -9410,9 +9417,9 @@
       <c r="E12" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="K12" s="31"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
       <c r="P12" s="13" t="s">
         <v>151</v>
       </c>
@@ -9454,9 +9461,9 @@
       <c r="E13" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="K13" s="31"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
       <c r="P13" s="13" t="s">
         <v>151</v>
       </c>
@@ -9498,9 +9505,9 @@
       <c r="E14" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="K14" s="31"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
       <c r="P14" s="13" t="s">
         <v>151</v>
       </c>
@@ -9539,9 +9546,9 @@
       <c r="E15" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="31"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
       <c r="P15" s="13" t="s">
         <v>31</v>
       </c>
@@ -9581,9 +9588,9 @@
       <c r="E16" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="K16" s="31"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
       <c r="P16" s="13" t="s">
         <v>151</v>
       </c>
@@ -9628,9 +9635,9 @@
       <c r="J17" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="K17" s="31"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
       <c r="P17" s="13" t="s">
         <v>151</v>
       </c>
@@ -9672,9 +9679,9 @@
       <c r="E18" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="K18" s="31"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
       <c r="P18" s="13" t="s">
         <v>151</v>
       </c>
@@ -9713,9 +9720,9 @@
       <c r="E19" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="K19" s="31"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
       <c r="P19" s="13" t="s">
         <v>163</v>
       </c>
@@ -9755,9 +9762,9 @@
       <c r="E20" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="K20" s="31"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
       <c r="P20" s="13" t="s">
         <v>151</v>
       </c>
@@ -9795,9 +9802,9 @@
       <c r="E21" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="K21" s="31"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
       <c r="P21" s="13" t="s">
         <v>151</v>
       </c>
@@ -9835,9 +9842,9 @@
       <c r="E22" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="K22" s="31"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
       <c r="P22" s="13" t="s">
         <v>151</v>
       </c>
@@ -9878,9 +9885,9 @@
       <c r="E23" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="K23" s="31"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
       <c r="P23" s="13" t="s">
         <v>151</v>
       </c>
@@ -9921,9 +9928,9 @@
       <c r="E24" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="K24" s="31"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
       <c r="P24" s="13" t="s">
         <v>151</v>
       </c>
@@ -9961,9 +9968,9 @@
       <c r="E25" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="K25" s="31"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
       <c r="P25" s="13" t="s">
         <v>163</v>
       </c>
@@ -10006,9 +10013,9 @@
       <c r="J26" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="K26" s="31"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
       <c r="P26" s="13" t="s">
         <v>31</v>
       </c>
@@ -10050,9 +10057,9 @@
       <c r="E27" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="K27" s="31"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
       <c r="P27" s="13" t="s">
         <v>190</v>
       </c>
@@ -10098,9 +10105,9 @@
       <c r="I28" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="K28" s="31"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="36"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
       <c r="P28" s="13" t="s">
         <v>157</v>
       </c>
@@ -10143,9 +10150,9 @@
       <c r="I29" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="K29" s="31"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
       <c r="P29" s="13" t="s">
         <v>157</v>
       </c>
@@ -10191,9 +10198,9 @@
       <c r="I30" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K30" s="31"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="36"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
       <c r="P30" s="13" t="s">
         <v>157</v>
       </c>
@@ -10242,9 +10249,9 @@
       <c r="I31" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="K31" s="31"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
       <c r="P31" s="13" t="s">
         <v>157</v>
       </c>
@@ -10289,9 +10296,9 @@
       <c r="J32" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="K32" s="31"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
       <c r="P32" s="13" t="s">
         <v>31</v>
       </c>
@@ -10337,9 +10344,9 @@
       <c r="J33" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="K33" s="31"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="36"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
       <c r="P33" s="13" t="s">
         <v>31</v>
       </c>
@@ -10382,9 +10389,9 @@
       <c r="I34" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="K34" s="31"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="36"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="46"/>
+      <c r="M34" s="46"/>
       <c r="P34" s="13" t="s">
         <v>157</v>
       </c>
@@ -10427,9 +10434,9 @@
       <c r="I35" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="K35" s="31"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="46"/>
       <c r="P35" s="13" t="s">
         <v>157</v>
       </c>
@@ -10475,9 +10482,9 @@
       <c r="J36" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="K36" s="31"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="36"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="46"/>
       <c r="P36" s="13" t="s">
         <v>31</v>
       </c>
@@ -10523,9 +10530,9 @@
       <c r="J37" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="K37" s="31"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="36"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="46"/>
       <c r="P37" s="13" t="s">
         <v>31</v>
       </c>
@@ -10568,9 +10575,9 @@
       <c r="I38" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="K38" s="31"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="36"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
       <c r="P38" s="13" t="s">
         <v>157</v>
       </c>
@@ -10610,9 +10617,9 @@
       <c r="E39" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K39" s="31"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="46"/>
       <c r="P39" s="13" t="s">
         <v>151</v>
       </c>
@@ -10652,9 +10659,9 @@
       <c r="E40" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="K40" s="31"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="36"/>
+      <c r="K40" s="43"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
       <c r="P40" s="13" t="s">
         <v>151</v>
       </c>
@@ -10697,9 +10704,9 @@
       <c r="I41" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="K41" s="31"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="36"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="46"/>
       <c r="P41" s="13" t="s">
         <v>157</v>
       </c>
@@ -10745,9 +10752,9 @@
       <c r="J42" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="K42" s="31"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="36"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="46"/>
       <c r="P42" s="13" t="s">
         <v>31</v>
       </c>
@@ -10793,9 +10800,9 @@
       <c r="J43" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="K43" s="31"/>
-      <c r="L43" s="36"/>
-      <c r="M43" s="36"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="46"/>
+      <c r="M43" s="46"/>
       <c r="P43" s="13" t="s">
         <v>31</v>
       </c>
@@ -10841,9 +10848,9 @@
       <c r="J44" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="K44" s="31"/>
-      <c r="L44" s="36"/>
-      <c r="M44" s="36"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="46"/>
+      <c r="M44" s="46"/>
       <c r="P44" s="13" t="s">
         <v>31</v>
       </c>
@@ -10889,9 +10896,9 @@
       <c r="J45" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="K45" s="31"/>
-      <c r="L45" s="36"/>
-      <c r="M45" s="36"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="46"/>
+      <c r="M45" s="46"/>
       <c r="P45" s="13" t="s">
         <v>31</v>
       </c>
@@ -10934,9 +10941,9 @@
       <c r="I46" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="K46" s="31"/>
-      <c r="L46" s="36"/>
-      <c r="M46" s="36"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="46"/>
+      <c r="M46" s="46"/>
       <c r="P46" s="13" t="s">
         <v>157</v>
       </c>
@@ -10979,9 +10986,9 @@
       <c r="I47" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="K47" s="31"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="36"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="46"/>
+      <c r="M47" s="46"/>
       <c r="P47" s="13" t="s">
         <v>157</v>
       </c>
@@ -11012,9 +11019,9 @@
       <c r="A48" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="K48" s="31"/>
-      <c r="L48" s="36"/>
-      <c r="M48" s="36"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="46"/>
+      <c r="M48" s="46"/>
       <c r="Z48" s="26"/>
       <c r="AA48" s="26"/>
       <c r="AB48" s="26"/>
@@ -11023,9 +11030,9 @@
       <c r="A49" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="K49" s="32"/>
-      <c r="L49" s="37"/>
-      <c r="M49" s="37"/>
+      <c r="K49" s="44"/>
+      <c r="L49" s="47"/>
+      <c r="M49" s="47"/>
       <c r="Z49" s="26"/>
       <c r="AA49" s="26"/>
       <c r="AB49" s="26"/>
@@ -11071,11 +11078,6 @@
     <sortCondition ref="D4:D49"/>
   </sortState>
   <mergeCells count="17">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:I1"/>
     <mergeCell ref="K4:K49"/>
     <mergeCell ref="Y1:AB1"/>
     <mergeCell ref="L4:L49"/>
@@ -11088,6 +11090,11 @@
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="J1:J3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:I1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11136,45 +11143,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="42" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="34"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="35"/>
       <c r="Z1" s="14"/>
       <c r="AA1" s="14"/>
       <c r="AB1" s="14"/>
@@ -11186,47 +11193,47 @@
       <c r="AH1" s="14"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33" t="s">
         <v>127</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="J2" s="43"/>
+      <c r="J2" s="40"/>
       <c r="K2" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="39" t="s">
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="39" t="s">
+      <c r="Q2" s="35"/>
+      <c r="R2" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="39" t="s">
+      <c r="S2" s="36"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="V2" s="33"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="39" t="s">
+      <c r="V2" s="36"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="Y2" s="34"/>
+      <c r="Y2" s="35"/>
       <c r="Z2" s="15"/>
       <c r="AA2" s="15"/>
       <c r="AB2" s="15"/>
@@ -11238,11 +11245,11 @@
       <c r="AH2" s="15"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="20" t="s">
         <v>128</v>
       </c>
@@ -11252,8 +11259,8 @@
       <c r="H3" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="44"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="41"/>
       <c r="K3" s="19" t="s">
         <v>148</v>
       </c>
@@ -13266,11 +13273,6 @@
     <sortCondition ref="A4"/>
   </sortState>
   <mergeCells count="14">
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="E1:I1"/>
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="E2:E3"/>
@@ -13280,6 +13282,11 @@
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="J1:J3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="E1:I1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15103,7 +15110,7 @@
         <v>1</v>
       </c>
       <c r="M13" s="5"/>
-      <c r="N13" s="45" t="s">
+      <c r="N13" s="48" t="s">
         <v>116</v>
       </c>
     </row>
@@ -15141,7 +15148,7 @@
         <v>1</v>
       </c>
       <c r="M14" s="5"/>
-      <c r="N14" s="45"/>
+      <c r="N14" s="48"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">

</xml_diff>